<commit_message>
updated boston with preliminary numbers
</commit_message>
<xml_diff>
--- a/assets/misc/2024/2024_Attendance.xlsx
+++ b/assets/misc/2024/2024_Attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve.jones\Documents\git\sqlsatwebsite\assets\misc\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB04FBC-772C-4435-9979-93CEB7F3E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ED18F3-ACEE-47ED-B1E4-B12CF2E0E719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22995" yWindow="870" windowWidth="21615" windowHeight="15015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Event</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>SQL Saturday Minnesota 2024 (1087)</t>
+  </si>
+  <si>
+    <t>SQL Saturday Boston 2024 (1086)</t>
   </si>
 </sst>
 </file>
@@ -496,19 +499,19 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -537,7 +540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>45318</v>
       </c>
@@ -555,7 +558,7 @@
         <v>0.63054187192118227</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>45332</v>
       </c>
@@ -573,7 +576,7 @@
         <v>0.39866369710467708</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>45360</v>
       </c>
@@ -591,7 +594,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>45387</v>
       </c>
@@ -609,7 +612,7 @@
         <v>0.50657894736842102</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>45388</v>
       </c>
@@ -627,7 +630,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>45402</v>
       </c>
@@ -648,7 +651,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>45409</v>
       </c>
@@ -667,7 +670,7 @@
         <v>0.44295302013422821</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>45409</v>
       </c>
@@ -685,7 +688,7 @@
         <v>-1.6722222222222223</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>45416</v>
       </c>
@@ -704,7 +707,7 @@
         <v>0.31928687196110211</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>45430</v>
       </c>
@@ -722,7 +725,7 @@
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>45444</v>
       </c>
@@ -740,7 +743,7 @@
         <v>0.4642857142857143</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>45465</v>
       </c>
@@ -758,7 +761,7 @@
         <v>-1.1139240506329113</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>45472</v>
       </c>
@@ -776,7 +779,7 @@
         <v>0.73039215686274506</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>45500</v>
       </c>
@@ -790,11 +793,11 @@
         <v>84</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E23" si="1">IF(C15=0,0,+(C15-D15)/C15)</f>
+        <f t="shared" ref="E15:E24" si="1">IF(C15=0,0,+(C15-D15)/C15)</f>
         <v>0.31147540983606559</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>45500</v>
       </c>
@@ -812,7 +815,7 @@
         <v>0.42511346444780634</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>45507</v>
       </c>
@@ -830,7 +833,7 @@
         <v>0.39130434782608697</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>45507</v>
       </c>
@@ -848,7 +851,7 @@
         <v>0.28358208955223879</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>45514</v>
       </c>
@@ -866,7 +869,7 @@
         <v>0.42148760330578511</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>45521</v>
       </c>
@@ -884,7 +887,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>45542</v>
       </c>
@@ -902,7 +905,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>45549</v>
       </c>
@@ -920,7 +923,7 @@
         <v>0.50881057268722463</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>45563</v>
       </c>
@@ -938,35 +941,46 @@
         <v>0.38589211618257263</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>45570</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24">
+        <v>250</v>
+      </c>
       <c r="D24">
-        <f>SUM(D2:D23)</f>
-        <v>4016</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
golive and cfs update
</commit_message>
<xml_diff>
--- a/assets/misc/2024/2024_Attendance.xlsx
+++ b/assets/misc/2024/2024_Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12403F06-38E1-4D39-BFA4-BAC96DBB7021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0A5808-D900-40DB-8D1B-D3F1BAD36783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="480" windowWidth="16860" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="705" windowWidth="26070" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
     <t>SQL Saturday Belo Horizonte 2024 (1097)</t>
   </si>
   <si>
-    <t>QSL Saturday Lima 2024 (1096)</t>
+    <t>SQL Saturday Lima 2024 (1096)</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,9 +1065,15 @@
       <c r="B29" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="C29">
+        <v>331</v>
+      </c>
+      <c r="D29">
+        <v>240</v>
+      </c>
       <c r="E29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.27492447129909364</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#764 adjust cfs note
</commit_message>
<xml_diff>
--- a/assets/misc/2024/2024_Attendance.xlsx
+++ b/assets/misc/2024/2024_Attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\git\sqlsatwebsite\assets\misc\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977C0B50-9022-467F-9EC7-58D0E2E73636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739E398D-86D2-4FFC-8FAB-7285FF1A49D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="510" windowWidth="26070" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="210" windowWidth="26070" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Event</t>
   </si>
@@ -159,13 +159,16 @@
   </si>
   <si>
     <t>SQL Saturday Houston 2024 (1098)</t>
+  </si>
+  <si>
+    <t>SQL Tuesday Sao Paulo 2024 (1099)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,13 +205,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,7 +228,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,7 +243,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -535,7 +532,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +826,7 @@
         <v>84</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E32" si="1">IF(C15=0,0,+(C15-D15)/C15)</f>
+        <f t="shared" ref="E15:E33" si="1">IF(C15=0,0,+(C15-D15)/C15)</f>
         <v>0.31147540983606559</v>
       </c>
     </row>
@@ -1133,8 +1130,23 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>45643</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33">
+        <v>152</v>
+      </c>
+      <c r="D33">
+        <v>81</v>
+      </c>
+      <c r="E33" s="8">
+        <f t="shared" si="1"/>
+        <v>0.46710526315789475</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">

</xml_diff>